<commit_message>
nova versao de plano de projetos e requisitos
</commit_message>
<xml_diff>
--- a/documentação/planilha/Tabela de controle de versionamento.xlsx
+++ b/documentação/planilha/Tabela de controle de versionamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">N da alteração </t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Repositorio Criado para o gerenciamento do projeto Next Page, armazenameto da documentação, codigos e a comunicação entre os integrantes do projeto.</t>
   </si>
   <si>
-    <t xml:space="preserve">aberto</t>
+    <t xml:space="preserve">Concluido</t>
   </si>
   <si>
     <t xml:space="preserve">Adição de plano de projeto</t>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Foi criado o plano de projeto, para a definição de funções, documentação do requisitos do projetos, que foram elicitados durantes as negociações, mantendo a descrição das praticas usadas, tecnologias e metodologias a serem usadas para o encaminhamento do projeto até a sua conclusão e entrega ao cliente.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concluido</t>
   </si>
   <si>
     <t xml:space="preserve">Elaboração da planilha de iCs</t>
@@ -173,48 +170,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,190 +411,190 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="8" t="n">
         <v>45898</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>45905</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="n">
-        <v>45905</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="7" t="n">
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>45907</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>